<commit_message>
changes in PQ questions
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\experiment_final\experiment_implementation\data\participant_questionnaire_toy_x_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A69E5E5-9657-634D-B075-082A88BE8A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E71E02-6BF4-4DEB-B5EB-4A394D5510F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_questionnaire_questi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
   <si>
     <t>pq_question_no</t>
   </si>
@@ -181,9 +181,6 @@
     <t>dialect</t>
   </si>
   <si>
-    <t xml:space="preserve">In a typical week, how much time do you spend reading in each type of material listed below in: </t>
-  </si>
-  <si>
     <t>Please exclude audiobooks.</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>other_reading_time</t>
   </si>
   <si>
-    <t>Do you read in any other language(s)?</t>
-  </si>
-  <si>
     <t>You can insert 4 languages.</t>
   </si>
   <si>
@@ -368,6 +362,15 @@
   </si>
   <si>
     <t>language_iso639_1_toy.xlsx</t>
+  </si>
+  <si>
+    <t>&gt;20 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you read in any other language(s) than </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a typical week, how much time do you spend reading each type of material listed below: </t>
   </si>
 </sst>
 </file>
@@ -1230,16 +1233,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.33203125" customWidth="1"/>
+    <col min="2" max="2" width="74.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1325,6 +1328,9 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
       <c r="L3" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1439,7 +1445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1459,7 +1465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -1479,7 +1485,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -1499,7 +1505,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1516,436 +1522,436 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" t="s">
         <v>53</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
         <v>54</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>61</v>
       </c>
-      <c r="G13" t="s">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
         <v>62</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>63</v>
       </c>
       <c r="O13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>66</v>
       </c>
       <c r="O14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>69</v>
       </c>
       <c r="O15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" t="s">
-        <v>62</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>72</v>
       </c>
       <c r="O16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" t="s">
-        <v>62</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
-        <v>75</v>
       </c>
       <c r="O17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" t="s">
-        <v>62</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>78</v>
       </c>
       <c r="O18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
         <v>79</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>81</v>
       </c>
       <c r="O19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
-        <v>84</v>
       </c>
       <c r="O20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" t="s">
+        <v>84</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
         <v>85</v>
       </c>
-      <c r="L21" t="s">
-        <v>86</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
         <v>88</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>89</v>
       </c>
-      <c r="D22" t="s">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
         <v>90</v>
-      </c>
-      <c r="E22" t="s">
-        <v>91</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>92</v>
       </c>
       <c r="O22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
         <v>93</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>94</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>95</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>96</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>97</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>98</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>99</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>100</v>
       </c>
-      <c r="J23" t="s">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
         <v>101</v>
-      </c>
-      <c r="K23" t="s">
-        <v>102</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>103</v>
       </c>
       <c r="O23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="L24" t="s">
         <v>105</v>
-      </c>
-      <c r="E24" t="s">
-        <v>106</v>
-      </c>
-      <c r="L24" t="s">
-        <v>107</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="L25" t="s">
         <v>105</v>
-      </c>
-      <c r="E25" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" t="s">
-        <v>107</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
         <v>112</v>
-      </c>
-      <c r="B26" t="s">
-        <v>113</v>
-      </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pq additional read lang, camera image
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cui/Documents/uzh/PhD/Projects/MultiplEYE/EXP/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cui/Documents/tmp/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A8397E-6F00-B64F-A0BF-56AA2C7CBA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85CC355-4C5E-7645-8764-E43FCC595102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_questionnaire_questi" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,14 @@
   <commentList>
     <comment ref="B22" authorId="0" shapeId="0" xr:uid="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     than [insert current language]?
 Reply:
     After 'than' the language of the experiment will be inserted automatically.
-</t>
+Reply:
+    As discussed in the multipleye slack channel, please substitute English with the language of the experiment , when translating.</t>
       </text>
     </comment>
   </commentList>
@@ -340,9 +341,6 @@
     <t>other_reading_time</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you read in any other language(s) than </t>
-  </si>
-  <si>
     <t>You can insert 4 languages.</t>
   </si>
   <si>
@@ -431,6 +429,9 @@
   </si>
   <si>
     <t>language_iso639_1_toy.xlsx</t>
+  </si>
+  <si>
+    <t>Do you read in any other language(s) than English?</t>
   </si>
 </sst>
 </file>
@@ -514,6 +515,7 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Stefan Frank (Gastgebruiker)" id="{F9E47CF5-FABA-A131-AD4D-74C918431CC5}" userId="uid-1704869221436" providerId="Teamlab"/>
   <person displayName="Anonymous" id="{3A5882BC-B3DC-DB74-617B-2B7A26713774}" userId="uid-1706708159632" providerId="Teamlab"/>
+  <person displayName="Cui Ding" id="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" userId="S::cui.ding@uzh.ch::c3b316e5-323e-462a-8a16-67367b714826" providerId="AD"/>
 </personList>
 </file>
 
@@ -755,6 +757,9 @@
     <text xml:space="preserve">After 'than' the language of the experiment will be inserted automatically.
 </text>
   </threadedComment>
+  <threadedComment ref="B22" dT="2024-11-02T19:53:12.74" personId="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" id="{690A537C-1B2C-B543-9CF7-E90870CDD549}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
+    <text>As discussed in the multipleye slack channel, please substitute English with the language of the experiment , when translating.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -763,7 +768,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,6 +781,8 @@
     <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="19.83203125" customWidth="1"/>
     <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="54" customWidth="1"/>
+    <col min="12" max="12" width="35.1640625" customWidth="1"/>
     <col min="13" max="13" width="31.6640625" customWidth="1"/>
     <col min="15" max="15" width="52.5" customWidth="1"/>
   </cols>
@@ -1020,7 +1027,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1040,7 +1047,7 @@
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1060,7 +1067,7 @@
         <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1080,7 +1087,7 @@
         <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1384,16 +1391,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="M22" t="s">
         <v>99</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" t="s">
         <v>100</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
@@ -1401,22 +1408,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>104</v>
       </c>
-      <c r="E23" t="s">
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
         <v>105</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
-        <v>106</v>
       </c>
       <c r="P23" t="s">
         <v>22</v>
@@ -1427,40 +1434,40 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
         <v>107</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>108</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>109</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>110</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>111</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>112</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>113</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>114</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>115</v>
       </c>
-      <c r="K24" t="s">
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
         <v>116</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>117</v>
       </c>
       <c r="P24" t="s">
         <v>22</v>
@@ -1471,25 +1478,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
         <v>118</v>
       </c>
-      <c r="C25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>119</v>
       </c>
-      <c r="E25" t="s">
+      <c r="M25" t="s">
         <v>120</v>
-      </c>
-      <c r="M25" t="s">
-        <v>121</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P25" t="s">
         <v>22</v>
@@ -1500,25 +1507,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
         <v>123</v>
       </c>
-      <c r="C26" t="s">
-        <v>124</v>
-      </c>
       <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" t="s">
         <v>119</v>
       </c>
-      <c r="E26" t="s">
+      <c r="M26" t="s">
         <v>120</v>
-      </c>
-      <c r="M26" t="s">
-        <v>121</v>
       </c>
       <c r="N26">
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P26" t="s">
         <v>22</v>
@@ -1526,16 +1533,16 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
         <v>126</v>
       </c>
-      <c r="B27" t="s">
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
         <v>127</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed pq 20 additional_read_language
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cui/Documents/tmp/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68165B30-E90F-FA48-990C-ADC362955AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE604F51-B8C4-AE4B-AD83-8D10D6A34916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,7 @@
 Comment:
     than [insert current language]?
 Reply:
-    After 'than' the language of the experiment will be inserted automatically.
-Reply:
-    As discussed in the multipleye slack channel, please substitute English with the language of the experiment , when translating.</t>
+    Hi, everyone who is going to translate this column, we don't need to specify any languages here. It is enough to say "do you read in any other language(s)?" A menu with language options is not needed because it will read the language options from the iso file directly. (Cui)</t>
       </text>
     </comment>
   </commentList>
@@ -431,7 +429,7 @@
     <t>language_iso639_1_toy.xlsx</t>
   </si>
   <si>
-    <t>Do you read in any other language(s) than English?</t>
+    <t>Do you read in any other language(s)?</t>
   </si>
 </sst>
 </file>
@@ -514,7 +512,6 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Stefan Frank (Gastgebruiker)" id="{F9E47CF5-FABA-A131-AD4D-74C918431CC5}" userId="uid-1704869221436" providerId="Teamlab"/>
-  <person displayName="Anonymous" id="{3A5882BC-B3DC-DB74-617B-2B7A26713774}" userId="uid-1706708159632" providerId="Teamlab"/>
   <person displayName="Cui Ding" id="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" userId="S::cui.ding@uzh.ch::c3b316e5-323e-462a-8a16-67367b714826" providerId="AD"/>
 </personList>
 </file>
@@ -753,12 +750,8 @@
     <text xml:space="preserve">than [insert current language]?
 </text>
   </threadedComment>
-  <threadedComment ref="B22" dT="2024-08-05T21:19:45.86" personId="{3A5882BC-B3DC-DB74-617B-2B7A26713774}" id="{49E0D68D-6D37-4C3E-04DC-0457A4320D4A}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
-    <text xml:space="preserve">After 'than' the language of the experiment will be inserted automatically.
-</text>
-  </threadedComment>
-  <threadedComment ref="B22" dT="2024-11-02T19:53:12.74" personId="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" id="{690A537C-1B2C-B543-9CF7-E90870CDD549}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
-    <text>As discussed in the multipleye slack channel, please substitute English with the language of the experiment , when translating.</text>
+  <threadedComment ref="B22" dT="2024-11-05T15:38:32.36" personId="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" id="{74697B6F-5D15-6F47-8BD5-5BA580D1B4BE}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
+    <text>Hi, everyone who is going to translate this column, we don't need to specify any languages here. It is enough to say "do you read in any other language(s)?" A menu with language options is not needed because it will read the language options from the iso file directly. (Cui)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -768,7 +761,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added isntructions on how to run pq separately
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/multipleye_questionnaire_questions_toy.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cui/Documents/tmp/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-experiment-implementation/experiment_implementation/data/participant_questionnaire_toy_x_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE604F51-B8C4-AE4B-AD83-8D10D6A34916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D22396-22AA-CC41-BBE8-45448568E13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multipleye_questionnaire_questi" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">multipleye_questionnaire_questi!$A$1:$P$27</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -25,7 +28,7 @@
     <author>tc={D353FB44-2422-FEF8-3AB3-E3F2443958F3}</author>
   </authors>
   <commentList>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -746,11 +749,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B22" dT="2024-07-15T15:00:22.01" personId="{F9E47CF5-FABA-A131-AD4D-74C918431CC5}" id="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
+  <threadedComment ref="B3" dT="2024-07-15T15:00:22.01" personId="{F9E47CF5-FABA-A131-AD4D-74C918431CC5}" id="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
     <text xml:space="preserve">than [insert current language]?
 </text>
   </threadedComment>
-  <threadedComment ref="B22" dT="2024-11-05T15:38:32.36" personId="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" id="{74697B6F-5D15-6F47-8BD5-5BA580D1B4BE}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
+  <threadedComment ref="B3" dT="2024-11-05T15:38:32.36" personId="{A0F657DF-FEB6-C44A-9013-0FF546126BA2}" id="{74697B6F-5D15-6F47-8BD5-5BA580D1B4BE}" parentId="{D353FB44-2422-FEF8-3AB3-E3F2443958F3}">
     <text>Hi, everyone who is going to translate this column, we don't need to specify any languages here. It is enough to say "do you read in any other language(s)?" A menu with language options is not needed because it will read the language options from the iso file directly. (Cui)</text>
   </threadedComment>
 </ThreadedComments>
@@ -761,7 +764,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,29 +834,32 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -861,123 +867,97 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>119</v>
       </c>
       <c r="M5" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
+        <v>119</v>
+      </c>
+      <c r="M6" t="s">
+        <v>120</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="P6" t="s">
         <v>22</v>
@@ -1014,50 +994,38 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
-      </c>
-      <c r="P8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
+      <c r="A9" t="s">
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>60</v>
-      </c>
-      <c r="P9" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>128</v>
@@ -1066,90 +1034,126 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
+      <c r="A11" t="s">
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="P11" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="P12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" t="s">
-        <v>68</v>
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
       </c>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>69</v>
+        <v>89</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>70</v>
+      <c r="A14">
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="P14" t="s">
         <v>22</v>
@@ -1157,10 +1161,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>72</v>
@@ -1181,39 +1185,53 @@
         <v>1</v>
       </c>
       <c r="O15" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="P15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" t="s">
-        <v>76</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="O16" t="s">
-        <v>83</v>
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="P16" t="s">
         <v>22</v>
@@ -1221,10 +1239,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>72</v>
@@ -1245,82 +1263,58 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="P17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>87</v>
+      <c r="A18">
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>90</v>
+      <c r="A19">
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="N19">
         <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="P19" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
@@ -1341,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="P20" t="s">
         <v>22</v>
@@ -1349,10 +1343,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
         <v>72</v>
@@ -1373,94 +1367,85 @@
         <v>1</v>
       </c>
       <c r="O21" t="s">
+        <v>92</v>
+      </c>
+      <c r="P21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" t="s">
         <v>98</v>
       </c>
-      <c r="P21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
-      <c r="M22" t="s">
-        <v>99</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>100</v>
+      <c r="P22" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" t="s">
-        <v>104</v>
+        <v>11</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M23" t="s">
+        <v>68</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>105</v>
-      </c>
-      <c r="P23" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H24" t="s">
-        <v>112</v>
-      </c>
-      <c r="I24" t="s">
-        <v>113</v>
-      </c>
-      <c r="J24" t="s">
-        <v>114</v>
-      </c>
-      <c r="K24" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="N24">
         <v>1</v>
       </c>
       <c r="O24" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="P24" t="s">
         <v>22</v>
@@ -1468,28 +1453,43 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
-      </c>
-      <c r="M25" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="F25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" t="s">
+        <v>115</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P25" t="s">
         <v>22</v>
@@ -1497,48 +1497,56 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>62</v>
+      </c>
+      <c r="P26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" t="s">
-        <v>119</v>
-      </c>
-      <c r="M26" t="s">
-        <v>120</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26" t="s">
-        <v>124</v>
-      </c>
-      <c r="P26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" t="s">
+        <v>26</v>
       </c>
       <c r="N27">
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>127</v>
+        <v>27</v>
+      </c>
+      <c r="P27" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P27" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
+      <sortCondition ref="O1:O27"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>